<commit_message>
feat: added balance success & failure flows, error_codes
</commit_message>
<xml_diff>
--- a/api/components/attributes/metro-card-recharge/metro-card-recharge.xlsx
+++ b/api/components/attributes/metro-card-recharge/metro-card-recharge.xlsx
@@ -36802,8 +36802,8 @@
       <c r="A30" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="B30" s="43" t="s">
-        <v>7</v>
+      <c r="B30" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>8</v>
@@ -36822,8 +36822,8 @@
       <c r="A31" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="B31" s="43" t="s">
-        <v>7</v>
+      <c r="B31" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>8</v>
@@ -36842,8 +36842,8 @@
       <c r="A32" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="B32" s="43" t="s">
-        <v>7</v>
+      <c r="B32" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>8</v>
@@ -40035,8 +40035,8 @@
       <c r="A49" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B49" s="43" t="s">
-        <v>7</v>
+      <c r="B49" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>8</v>
@@ -40076,8 +40076,8 @@
       <c r="A50" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B50" s="43" t="s">
-        <v>7</v>
+      <c r="B50" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>8</v>
@@ -40117,8 +40117,8 @@
       <c r="A51" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B51" s="43" t="s">
-        <v>7</v>
+      <c r="B51" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>8</v>
@@ -40158,8 +40158,8 @@
       <c r="A52" s="66" t="s">
         <v>243</v>
       </c>
-      <c r="B52" s="43" t="s">
-        <v>7</v>
+      <c r="B52" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>8</v>
@@ -42786,8 +42786,8 @@
       <c r="A30" s="66" t="s">
         <v>243</v>
       </c>
-      <c r="B30" s="43" t="s">
-        <v>7</v>
+      <c r="B30" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>8</v>
@@ -42827,8 +42827,8 @@
       <c r="A31" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B31" s="43" t="s">
-        <v>7</v>
+      <c r="B31" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>8</v>
@@ -42868,8 +42868,8 @@
       <c r="A32" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B32" s="43" t="s">
-        <v>7</v>
+      <c r="B32" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>8</v>
@@ -42909,8 +42909,8 @@
       <c r="A33" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B33" s="43" t="s">
-        <v>7</v>
+      <c r="B33" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>8</v>
@@ -42950,8 +42950,8 @@
       <c r="A34" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B34" s="43" t="s">
-        <v>7</v>
+      <c r="B34" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>8</v>
@@ -42991,8 +42991,8 @@
       <c r="A35" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B35" s="43" t="s">
-        <v>7</v>
+      <c r="B35" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>8</v>
@@ -43032,8 +43032,8 @@
       <c r="A36" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B36" s="43" t="s">
-        <v>7</v>
+      <c r="B36" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>8</v>
@@ -46836,8 +46836,8 @@
       <c r="A51" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B51" s="43" t="s">
-        <v>7</v>
+      <c r="B51" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>8</v>
@@ -46877,8 +46877,8 @@
       <c r="A52" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B52" s="43" t="s">
-        <v>7</v>
+      <c r="B52" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>8</v>
@@ -46918,8 +46918,8 @@
       <c r="A53" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B53" s="43" t="s">
-        <v>7</v>
+      <c r="B53" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>8</v>
@@ -46959,8 +46959,8 @@
       <c r="A54" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B54" s="43" t="s">
-        <v>7</v>
+      <c r="B54" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>8</v>
@@ -47820,8 +47820,8 @@
       <c r="A75" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B75" s="43" t="s">
-        <v>7</v>
+      <c r="B75" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>8</v>
@@ -47861,8 +47861,8 @@
       <c r="A76" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B76" s="43" t="s">
-        <v>7</v>
+      <c r="B76" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>8</v>
@@ -47902,8 +47902,8 @@
       <c r="A77" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B77" s="43" t="s">
-        <v>7</v>
+      <c r="B77" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>8</v>

</xml_diff>